<commit_message>
Taking testing data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testingDataExcel.xlsx
+++ b/src/test/resources/testingDataExcel.xlsx
@@ -4,28 +4,77 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="28356" windowHeight="12192"/>
+    <workbookView xWindow="192" yWindow="48" windowWidth="23256" windowHeight="12192"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>driver.name</t>
+  </si>
+  <si>
+    <t>driver.lastName</t>
+  </si>
+  <si>
+    <t>driver.email</t>
+  </si>
+  <si>
+    <t>driver.phone</t>
+  </si>
+  <si>
+    <t>vehicle.license</t>
+  </si>
+  <si>
+    <t>vehicle.model</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>automation1@mailinator.com</t>
+  </si>
+  <si>
+    <t>9999999998</t>
+  </si>
+  <si>
+    <t>2342367</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Caravan</t>
+  </si>
+  <si>
+    <t>vehicle.cab</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>vehicle.make</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +82,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,14 +121,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,44 +452,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding scenarios to driver app feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testingDataExcel.xlsx
+++ b/src/test/resources/testingDataExcel.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="23256" windowHeight="12192"/>
+    <workbookView xWindow="192" yWindow="48" windowWidth="23256" windowHeight="12192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Test</t>
   </si>
@@ -68,6 +69,18 @@
   </si>
   <si>
     <t>vehicle.make</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>automation_1629417720060@mailinator.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ChangeMe@.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -768,4 +781,247 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding missing escenarios for new fares
</commit_message>
<xml_diff>
--- a/src/test/resources/testingDataExcel.xlsx
+++ b/src/test/resources/testingDataExcel.xlsx
@@ -8,21 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RamonPC\Desktop\Ramon\Workspace_mobile22\QAWebAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C2F216-F7ED-438A-AEC1-DE041E1D6445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7FAB32-77A2-4F81-B2B0-B5C013904343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
     <sheet name="Data3" sheetId="3" r:id="rId3"/>
+    <sheet name="Data4" sheetId="4" r:id="rId4"/>
+    <sheet name="Data5" sheetId="5" r:id="rId5"/>
+    <sheet name="Data6" sheetId="6" r:id="rId6"/>
+    <sheet name="Data7" sheetId="7" r:id="rId7"/>
+    <sheet name="Data8" sheetId="8" r:id="rId8"/>
+    <sheet name="Data9" sheetId="9" r:id="rId9"/>
+    <sheet name="Data10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="68">
   <si>
     <t>Test</t>
   </si>
@@ -99,9 +106,6 @@
     <t>PickupLocation</t>
   </si>
   <si>
-    <t>Fare</t>
-  </si>
-  <si>
     <t>Timing</t>
   </si>
   <si>
@@ -111,10 +115,124 @@
     <t>Henry Villas Zoo</t>
   </si>
   <si>
-    <t>NEXT AVAILABLE</t>
-  </si>
-  <si>
     <t>Wheelchair</t>
+  </si>
+  <si>
+    <t>SCHEDULED</t>
+  </si>
+  <si>
+    <t>RiderFirstName</t>
+  </si>
+  <si>
+    <t>RiderLastName</t>
+  </si>
+  <si>
+    <t>RiderPhone</t>
+  </si>
+  <si>
+    <t>RiderEmail</t>
+  </si>
+  <si>
+    <t>Wheelchair Fare</t>
+  </si>
+  <si>
+    <t>8888888888</t>
+  </si>
+  <si>
+    <t>Automation_Wheelchair@mailinator.com</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>BaseFare</t>
+  </si>
+  <si>
+    <t>MileageExtraRate</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>MileageIncluded</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Can use 0 in case it is less than mileageIncluded</t>
+  </si>
+  <si>
+    <t>Fiserv Forum milwaukee</t>
+  </si>
+  <si>
+    <t>Wheelchair Extra</t>
+  </si>
+  <si>
+    <t>Automation_Wheelchair2@mailinator.com</t>
+  </si>
+  <si>
+    <t>76.68</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Hospital Extra</t>
+  </si>
+  <si>
+    <t>Automation_Hospital2@mailinator.com</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Automation_Hospital1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Stretcher</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Automation_Stretcher1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Stretcher extra</t>
+  </si>
+  <si>
+    <t>Automation_Stretcher2@mailinator.com</t>
+  </si>
+  <si>
+    <t>Hospital Base</t>
+  </si>
+  <si>
+    <t>37.5</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Holiday extra</t>
+  </si>
+  <si>
+    <t>Holiday Base</t>
+  </si>
+  <si>
+    <t>Automation_Holiday1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Automation_Holiday2@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -161,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +295,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +335,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,6 +348,13 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -883,6 +1014,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93806122-8428-4256-9F83-A75249CF3251}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{40F3452E-CB79-450C-986C-37634B0B7062}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G23"/>
@@ -1128,20 +1394,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C6B6DE-C68A-417E-86A3-060BF3462C4C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1149,48 +1415,924 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3">
         <v>27.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{6F5910AD-373B-42B3-8507-DD1F52CE8465}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF70F73-A0E6-4474-84B2-7B1C2396D6E8}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{07B13DB5-CB94-48FD-8401-9CE1D13B8C2B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E15675C-EBA3-413F-BA60-D0D79546E0FE}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{D4B27D02-99DA-4D36-8F9F-08F9574C7EB5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDABCBC-BF3C-4747-95D3-ABCF0A62D3C4}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{48D764E1-8741-44EF-957E-0DAF34CAC1F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C87956-02B9-49BB-B2AE-4A06812BC880}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{C7686211-549F-4518-940D-37B202CFB63D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD502EC-1A70-4E34-AD6C-D22944A1F38A}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{13812C55-DD34-4530-A89F-BBB3F4824A1F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FDD4E0-107B-44D7-929C-CDBBCDFCA60D}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{19A50D7C-4265-42D4-A0D7-F68F32B6E0B7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>